<commit_message>
updated both client and server design
</commit_message>
<xml_diff>
--- a/docs/status.xlsx
+++ b/docs/status.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="145">
   <si>
     <t>#</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Function sentCredits(int credits) to transmit current credit load</t>
   </si>
   <si>
-    <t>Add case to process player health, credit, endgame and newactordata packets</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
   </si>
   <si>
     <t>Protocol</t>
-  </si>
-  <si>
-    <t>Agree on packet info for health, credits, gameover, character (actor) info.</t>
   </si>
   <si>
     <t>User Documentation</t>
@@ -394,9 +388,6 @@
     <t>Add int health, boolean inBridge, int lastClass, float distFromLastEx, boolean sick, int credits, int lastClassAttended</t>
   </si>
   <si>
-    <t>Add a processCollision(Integer id) function which handles collisions with all other objects.  Update the following accordingly: health, speed, lastClass, distFromLastEx, sick, credits.  Return 1 if game won, 0 otherwise.</t>
-  </si>
-  <si>
     <t>Transmit game over when gamestate changes to gameover (check winner)</t>
   </si>
   <si>
@@ -482,6 +473,33 @@
   </si>
   <si>
     <t>Add function GAME_STATE checkState(), boolean checkState(GAME_STATE s)</t>
+  </si>
+  <si>
+    <t>Add String message, String lastClassAttended</t>
+  </si>
+  <si>
+    <t>Add int health, int credits</t>
+  </si>
+  <si>
+    <t>Modify render function to display health and credits and only render if actor is on screen</t>
+  </si>
+  <si>
+    <t>Add case to process player health, credit, gameover, newactordata, last class attended, message packets</t>
+  </si>
+  <si>
+    <t>Modify render function to display health, credits, last class attended and message</t>
+  </si>
+  <si>
+    <t>Add function getLastClass()</t>
+  </si>
+  <si>
+    <t>Add function getMessage()</t>
+  </si>
+  <si>
+    <t>Add a processCollision(Integer id) function which handles collisions with all other objects.  Update the following accordingly: health, speed, lastClass, distFromLastEx, sick, credits.  Return a message stating what the collision was "interacted with professor" or "attended CS101".  This function also changes the gamestate to gameover and sets the winner string in GlobalGameLogic if necessary.  It also resets distFromLastCollision to 0.</t>
+  </si>
+  <si>
+    <t>Agree on packet info for health, credits, speed, gameover with name, character (actor) info, last class attended (string), message (string)</t>
   </si>
 </sst>
 </file>
@@ -669,7 +687,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -967,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1002,7 +1034,7 @@
     <row r="2" spans="1:5">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>30</v>
@@ -1010,20 +1042,24 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="18"/>
+        <v>3</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
@@ -1034,7 +1070,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="18"/>
     </row>
@@ -1047,7 +1083,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E5" s="18"/>
     </row>
@@ -1060,7 +1096,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E6" s="18"/>
     </row>
@@ -1073,7 +1109,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="18"/>
     </row>
@@ -1086,7 +1122,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E8" s="18"/>
     </row>
@@ -1099,7 +1135,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="18"/>
     </row>
@@ -1112,7 +1148,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E10" s="18"/>
     </row>
@@ -1125,39 +1161,39 @@
         <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="18"/>
+        <v>21</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>22</v>
+      </c>
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>25</v>
@@ -1166,43 +1202,43 @@
         <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>25</v>
@@ -1214,202 +1250,198 @@
         <v>9</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="18"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="6" t="s">
+      <c r="C23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3"/>
+      <c r="B24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" s="18" t="s">
+      <c r="C24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30">
-      <c r="A24" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="6" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30">
-      <c r="A25" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="3"/>
-      <c r="B28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3" t="s">
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>25</v>
@@ -1418,218 +1450,214 @@
         <v>50</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30">
+      <c r="A34" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="18"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="F31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
+      <c r="B40" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="3" t="s">
+      <c r="B41" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="18"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="18"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="20" t="s">
+      <c r="B42" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="45">
-      <c r="A39" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30">
-      <c r="A41" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30">
-      <c r="A43" s="3" t="s">
-        <v>118</v>
+      <c r="E42" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="90">
+      <c r="A43" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>25</v>
@@ -1641,12 +1669,12 @@
         <v>13</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>25</v>
@@ -1655,32 +1683,32 @@
         <v>29</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="45">
-      <c r="A45" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B45" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30">
+      <c r="A45" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>3</v>
+      <c r="D45" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>25</v>
@@ -1692,46 +1720,46 @@
         <v>13</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="60">
-      <c r="A47" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="30">
+      <c r="A47" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>4</v>
+      <c r="D47" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="45">
       <c r="A49" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>25</v>
@@ -1740,66 +1768,66 @@
         <v>29</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30">
+      <c r="A50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="60">
+      <c r="A51" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30">
-      <c r="A50" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="E51" s="18" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B52" s="3" t="s">
+      <c r="A52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="45">
+      <c r="A53" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>25</v>
@@ -1811,11 +1839,11 @@
         <v>4</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30">
+      <c r="A54" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -1825,10 +1853,10 @@
         <v>29</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1842,13 +1870,13 @@
         <v>29</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="6" t="s">
         <v>115</v>
       </c>
@@ -1859,134 +1887,134 @@
         <v>29</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="18" t="s">
+      <c r="E58" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E62" s="18" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="30">
-      <c r="A58" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="30">
-      <c r="A61" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B63" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>7</v>
+      <c r="D63" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>25</v>
@@ -1995,15 +2023,15 @@
         <v>29</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="30">
       <c r="A65" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>25</v>
@@ -2012,15 +2040,15 @@
         <v>29</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>25</v>
@@ -2029,15 +2057,15 @@
         <v>29</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>25</v>
@@ -2049,29 +2077,29 @@
         <v>7</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>25</v>
@@ -2083,12 +2111,12 @@
         <v>7</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="3" t="s">
-        <v>117</v>
+      <c r="A70" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>25</v>
@@ -2100,12 +2128,12 @@
         <v>7</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>104</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="3" t="s">
-        <v>117</v>
+      <c r="A71" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>25</v>
@@ -2117,29 +2145,29 @@
         <v>7</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B72" s="3" t="s">
+      <c r="A72" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>25</v>
@@ -2151,78 +2179,146 @@
         <v>7</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>132</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B74" s="6" t="s">
+      <c r="A74" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E74" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="45">
-      <c r="A75" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75" s="6" t="s">
+      <c r="E78" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="45">
+      <c r="A79" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E75" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30">
-      <c r="A76" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D76" s="6" t="s">
+      <c r="E79" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="30">
+      <c r="A80" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E76" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B77" s="3" t="s">
+      <c r="E80" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D77" s="3" t="s">
+      <c r="C81" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="18"/>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="B78" s="6"/>
-      <c r="D78" s="6"/>
+      <c r="E81" s="18"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="B82" s="6"/>
+      <c r="D82" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:F76">
@@ -2232,7 +2328,7 @@
     <sortCondition ref="E2:E76"/>
   </sortState>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2257,114 +2353,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1">
       <c r="A2" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="10" customFormat="1" ht="30">
       <c r="A4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
       <c r="A5" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="10" customFormat="1" ht="30">
       <c r="A6" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="10" customFormat="1" ht="30">
       <c r="A8" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>77</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="10" customFormat="1" ht="30">
       <c r="A10" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="45">
       <c r="A11" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="10" customFormat="1" ht="30">
       <c r="A12" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
       <c r="A13" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="10" customFormat="1" ht="30">
       <c r="A14" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>